<commit_message>
add rounds to decimal values
</commit_message>
<xml_diff>
--- a/register/uncompletedRegister.xlsx
+++ b/register/uncompletedRegister.xlsx
@@ -378,7 +378,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BE2"/>
+  <dimension ref="A1:AX2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -391,347 +391,305 @@
         <v>NUM_RESEC</v>
       </c>
       <c r="C1" s="1" t="str">
+        <v>NUM_PAC</v>
+      </c>
+      <c r="D1" s="1" t="str">
         <v>NOMBRE</v>
       </c>
-      <c r="D1" s="1" t="str">
+      <c r="E1" s="1" t="str">
         <v>APELLIDO1</v>
       </c>
-      <c r="E1" s="1" t="str">
+      <c r="F1" s="1" t="str">
         <v>APELLIDO2</v>
       </c>
-      <c r="F1" s="1" t="str">
+      <c r="G1" s="1" t="str">
         <v>SAP</v>
       </c>
-      <c r="G1" s="1" t="str">
+      <c r="H1" s="1" t="str">
         <v>COMITE</v>
       </c>
-      <c r="H1" s="1" t="str">
+      <c r="I1" s="1" t="str">
         <v>SEXO</v>
       </c>
-      <c r="I1" s="1" t="str">
+      <c r="J1" s="1" t="str">
         <v>EDAT</v>
       </c>
-      <c r="J1" s="1" t="str">
+      <c r="K1" s="1" t="str">
         <v>PES</v>
       </c>
-      <c r="K1" s="1" t="str">
-        <v>Talla</v>
-      </c>
       <c r="L1" s="1" t="str">
-        <v>IMC</v>
+        <v>DATAIQCOLON</v>
       </c>
       <c r="M1" s="1" t="str">
-        <v>ASA</v>
+        <v>EPPO</v>
       </c>
       <c r="N1" s="1" t="str">
-        <v>DATAIQCOLON</v>
+        <v>DATAHEP</v>
       </c>
       <c r="O1" s="1" t="str">
-        <v>EPPO</v>
+        <v>RESMAY_MEN_ampli</v>
       </c>
       <c r="P1" s="1" t="str">
-        <v>DATAHEP</v>
+        <v>TecnicaQuir_descripció</v>
       </c>
       <c r="Q1" s="1" t="str">
-        <v>RESMAY_MEN_ampli</v>
+        <v>VIA ACCES</v>
       </c>
       <c r="R1" s="1" t="str">
-        <v>TecnicaQuir_descripció</v>
+        <v>RF</v>
       </c>
       <c r="S1" s="1" t="str">
-        <v>VIA ACCES</v>
+        <v>mw</v>
       </c>
       <c r="T1" s="1" t="str">
-        <v>RF</v>
+        <v>Val R cir</v>
       </c>
       <c r="U1" s="1" t="str">
-        <v>mw</v>
+        <v>BILOBUL</v>
       </c>
       <c r="V1" s="1" t="str">
-        <v>Val R cir</v>
+        <v>RES2</v>
       </c>
       <c r="W1" s="1" t="str">
-        <v>NMETIMAGpre</v>
+        <v>RES3</v>
       </c>
       <c r="X1" s="1" t="str">
-        <v>MIDA MH  IMATGE</v>
+        <v>CIRSIMCOLON</v>
       </c>
       <c r="Y1" s="1" t="str">
-        <v>BILOBUL</v>
+        <v>TIPUSCIRSIMCOL</v>
       </c>
       <c r="Z1" s="1" t="str">
-        <v>RES2</v>
+        <v>TIPUS CIRCOLONSIM</v>
       </c>
       <c r="AA1" s="1" t="str">
-        <v>RES3</v>
+        <v>MORBIDITAT</v>
       </c>
       <c r="AB1" s="1" t="str">
-        <v>CIRSIMCOLON</v>
+        <v>GRAU CLAVIEN</v>
       </c>
       <c r="AC1" s="1" t="str">
-        <v>TIPUSCIRSIMCOL</v>
+        <v>NMETAP</v>
       </c>
       <c r="AD1" s="1" t="str">
-        <v>TIPUS CIRCOLONSIM</v>
+        <v>MIDA AP</v>
       </c>
       <c r="AE1" s="1" t="str">
-        <v>MORBIDITAT</v>
+        <v>MARGEN</v>
       </c>
       <c r="AF1" s="1" t="str">
-        <v>GRAU CLAVIEN</v>
+        <v>INVMARG</v>
       </c>
       <c r="AG1" s="1" t="str">
-        <v>CCIndex</v>
+        <v>TRATMARGE</v>
       </c>
       <c r="AH1" s="1" t="str">
-        <v>NMETAP</v>
+        <v>DATA ULT CONT</v>
       </c>
       <c r="AI1" s="1" t="str">
-        <v>MIDA AP</v>
+        <v>ALPSS</v>
       </c>
       <c r="AJ1" s="1" t="str">
-        <v>MARGEN</v>
+        <v>INSUFHEP isgls</v>
       </c>
       <c r="AK1" s="1" t="str">
-        <v>INVMARG</v>
+        <v>ESTAT</v>
       </c>
       <c r="AL1" s="1" t="str">
-        <v>TRATMARGE</v>
+        <v>FISTBILI</v>
       </c>
       <c r="AM1" s="1" t="str">
-        <v>DATA ULT CONT</v>
+        <v>Grau IH</v>
       </c>
       <c r="AN1" s="1" t="str">
-        <v>ALPSS</v>
+        <v>INF ESPAI</v>
       </c>
       <c r="AO1" s="1" t="str">
-        <v>INSUFHEP isgls</v>
+        <v>HEMOPER</v>
       </c>
       <c r="AP1" s="1" t="str">
-        <v>ESTAT</v>
+        <v>ASCITIS</v>
       </c>
       <c r="AQ1" s="1" t="str">
-        <v>FISTBILI</v>
+        <v>REIQ</v>
       </c>
       <c r="AR1" s="1" t="str">
-        <v>Grau IH</v>
+        <v>MORTALITAT</v>
       </c>
       <c r="AS1" s="1" t="str">
-        <v>INF ESPAI</v>
+        <v>Causa REIQ</v>
       </c>
       <c r="AT1" s="1" t="str">
-        <v>HEMOPER</v>
+        <v>RECIDIVA</v>
       </c>
       <c r="AU1" s="1" t="str">
-        <v>ASCITIS</v>
+        <v>RECHEP</v>
       </c>
       <c r="AV1" s="1" t="str">
-        <v>REIQ</v>
+        <v>RECPUL</v>
       </c>
       <c r="AW1" s="1" t="str">
-        <v>MORTALITAT</v>
+        <v>timestamp</v>
       </c>
       <c r="AX1" s="1" t="str">
-        <v>Causa REIQ</v>
-      </c>
-      <c r="AY1" s="1" t="str">
-        <v>RECIDIVA</v>
-      </c>
-      <c r="AZ1" s="1" t="str">
-        <v>RECHEP</v>
-      </c>
-      <c r="BA1" s="1" t="str">
-        <v>RECPUL</v>
-      </c>
-      <c r="BB1" s="1" t="str">
-        <v>ESTADA</v>
-      </c>
-      <c r="BC1" s="1" t="str">
-        <v>GRAU FB</v>
-      </c>
-      <c r="BD1" s="1" t="str">
-        <v>timestamp</v>
-      </c>
-      <c r="BE1" s="1" t="str">
         <v>errorType</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="str">
-        <v>Hepatectomia dreta</v>
+        <v>Resecció/ns limitada/es</v>
       </c>
       <c r="B2" s="1">
-        <v>1695</v>
-      </c>
-      <c r="C2" s="1" t="str">
-        <v>Jordi</v>
+        <v>1669</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1529</v>
       </c>
       <c r="D2" s="1" t="str">
-        <v>Morillas2</v>
+        <v>Salvador</v>
       </c>
       <c r="E2" s="1" t="str">
-        <v>Esteban2</v>
-      </c>
-      <c r="F2" s="1">
-        <v>13296015</v>
-      </c>
-      <c r="G2" s="1" t="str">
+        <v>Monte</v>
+      </c>
+      <c r="F2" s="1" t="str">
+        <v>Peiro</v>
+      </c>
+      <c r="G2" s="1">
+        <v>13005406</v>
+      </c>
+      <c r="H2" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="I2" s="1" t="str">
+        <v>Home</v>
+      </c>
+      <c r="J2" s="1" t="str">
+        <v>60</v>
+      </c>
+      <c r="K2" s="1" t="str">
+        <v/>
+      </c>
+      <c r="L2" s="2">
+        <v>43525</v>
+      </c>
+      <c r="M2" s="1" t="str">
+        <v/>
+      </c>
+      <c r="N2" s="2">
+        <v>43679</v>
+      </c>
+      <c r="O2" s="1" t="str">
+        <v>Resecció Menor (&lt;3 segm)</v>
+      </c>
+      <c r="P2" s="1" t="str">
+        <v>bisegm 2/3 i 4 RL r0 una d'elles</v>
+      </c>
+      <c r="Q2" s="1" t="str">
+        <v>Oberta</v>
+      </c>
+      <c r="R2" s="1" t="str">
         <v>No</v>
       </c>
-      <c r="H2" s="1" t="str">
-        <v/>
-      </c>
-      <c r="I2" s="1" t="str">
-        <v/>
-      </c>
-      <c r="J2" s="1" t="str">
-        <v>79</v>
-      </c>
-      <c r="K2" s="1">
-        <v>178</v>
-      </c>
-      <c r="L2" s="1">
-        <v>25</v>
-      </c>
-      <c r="M2" s="1">
-        <v>3</v>
-      </c>
-      <c r="N2" s="2">
-        <v>43446</v>
-      </c>
-      <c r="O2" s="1" t="str">
+      <c r="S2" s="1" t="str">
         <v>No</v>
       </c>
-      <c r="P2" s="2">
-        <v>43858</v>
-      </c>
-      <c r="Q2" s="1" t="str">
-        <v>Resecció Major (&gt;= 3 segm)</v>
-      </c>
-      <c r="R2" s="1" t="str">
-        <v>hepatectomia dreta</v>
-      </c>
-      <c r="S2" s="1" t="str">
-        <v>Oberta</v>
-      </c>
       <c r="T2" s="1" t="str">
-        <v>Si, com a primer temps quirúrgic</v>
+        <v>Impressió R1</v>
       </c>
       <c r="U2" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="V2" s="1" t="str">
         <v>No</v>
       </c>
-      <c r="V2" s="1" t="str">
-        <v>Impressió R1</v>
-      </c>
-      <c r="W2" s="1">
-        <v>1</v>
-      </c>
-      <c r="X2" s="1">
-        <v>3</v>
+      <c r="W2" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="X2" s="1" t="str">
+        <v>No</v>
       </c>
       <c r="Y2" s="1" t="str">
+        <v/>
+      </c>
+      <c r="Z2" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AA2" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AB2" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AC2" s="1">
+        <v>7</v>
+      </c>
+      <c r="AD2" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="AE2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF2" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AG2" s="1" t="str">
+        <v>aquamantis</v>
+      </c>
+      <c r="AH2" s="2">
+        <v>44525</v>
+      </c>
+      <c r="AI2" s="1" t="str">
         <v>No</v>
       </c>
-      <c r="Z2" s="1" t="str">
+      <c r="AJ2" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AK2" s="1" t="str">
+        <v>Viu</v>
+      </c>
+      <c r="AL2" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AM2" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AN2" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AO2" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AP2" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AQ2" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AR2" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AS2" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AT2" s="1" t="str">
         <v>Si</v>
       </c>
-      <c r="AA2" s="1" t="str">
-        <v>No</v>
-      </c>
-      <c r="AB2" s="1" t="str">
-        <v>No</v>
-      </c>
-      <c r="AC2" s="1" t="str">
-        <v/>
-      </c>
-      <c r="AD2" s="1" t="str">
-        <v/>
-      </c>
-      <c r="AE2" s="1" t="str">
+      <c r="AU2" s="1" t="str">
         <v>Si</v>
-      </c>
-      <c r="AF2" s="1" t="str">
-        <v>IIIb</v>
-      </c>
-      <c r="AG2" s="1">
-        <v>61</v>
-      </c>
-      <c r="AH2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AI2" s="1">
-        <v>3</v>
-      </c>
-      <c r="AJ2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AK2" s="1" t="str">
-        <v>Si</v>
-      </c>
-      <c r="AL2" s="1" t="str">
-        <v>ampliacio quirurgica</v>
-      </c>
-      <c r="AM2" s="2">
-        <v>43983</v>
-      </c>
-      <c r="AN2" s="1" t="str">
-        <v>No</v>
-      </c>
-      <c r="AO2" s="1" t="str">
-        <v>No</v>
-      </c>
-      <c r="AP2" s="1" t="str">
-        <v>Viu</v>
-      </c>
-      <c r="AQ2" s="1" t="str">
-        <v>Si</v>
-      </c>
-      <c r="AR2" s="1" t="str">
-        <v/>
-      </c>
-      <c r="AS2" s="1" t="str">
-        <v>Si</v>
-      </c>
-      <c r="AT2" s="1" t="str">
-        <v>No</v>
-      </c>
-      <c r="AU2" s="1" t="str">
-        <v>No</v>
       </c>
       <c r="AV2" s="1" t="str">
         <v>Si</v>
       </c>
-      <c r="AW2" s="1" t="str">
-        <v>No</v>
+      <c r="AW2" s="2">
+        <v>44599.83927568287</v>
       </c>
       <c r="AX2" s="1" t="str">
-        <v>oclusió, peritonitis fecaoidea</v>
-      </c>
-      <c r="AY2" s="1" t="str">
-        <v>No</v>
-      </c>
-      <c r="AZ2" s="1" t="str">
-        <v>No</v>
-      </c>
-      <c r="BA2" s="1" t="str">
-        <v>No</v>
-      </c>
-      <c r="BB2" s="1">
-        <v>55</v>
-      </c>
-      <c r="BC2" s="1">
-        <v>2</v>
-      </c>
-      <c r="BD2" s="2">
-        <v>44599.650579270834</v>
-      </c>
-      <c r="BE2" s="1" t="str">
         <v>Falta alguna variable, revisar</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:BE2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AX2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
problems with server, checking types
</commit_message>
<xml_diff>
--- a/register/uncompletedRegister.xlsx
+++ b/register/uncompletedRegister.xlsx
@@ -10,9 +10,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -378,7 +379,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BF3"/>
+  <dimension ref="A1:BE9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -555,338 +556,964 @@
       <c r="BE1" s="1" t="str">
         <v>ESTADA</v>
       </c>
-      <c r="BF1" s="1" t="str">
-        <v>GRAU FB</v>
-      </c>
     </row>
-    <row r="2">
-      <c r="A2" s="1" t="str">
+    <row r="4">
+      <c r="A4" s="1" t="str">
         <v>Resecció/ns limitada/es</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B4" s="1">
         <v>1669</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C4" s="1">
         <v>1529</v>
       </c>
-      <c r="D2" s="1" t="str">
+      <c r="D4" s="1" t="str">
         <v>Salvador</v>
       </c>
-      <c r="E2" s="1" t="str">
+      <c r="E4" s="1" t="str">
         <v>Monte</v>
       </c>
-      <c r="F2" s="1" t="str">
+      <c r="F4" s="1" t="str">
         <v>Peiro</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G4" s="1">
         <v>13005406</v>
       </c>
-      <c r="H2" s="1" t="str">
-        <v>Si</v>
-      </c>
-      <c r="I2" s="1" t="str">
+      <c r="H4" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="I4" s="1" t="str">
         <v>Home</v>
       </c>
-      <c r="J2" s="1" t="str">
+      <c r="J4" s="1" t="str">
         <v>60</v>
       </c>
-      <c r="K2" s="1" t="str">
-        <v/>
-      </c>
-      <c r="L2" s="2">
+      <c r="K4" s="1" t="str">
+        <v/>
+      </c>
+      <c r="L4" s="2">
         <v>43525</v>
       </c>
-      <c r="M2" s="1" t="str">
-        <v/>
-      </c>
-      <c r="N2" s="2">
+      <c r="M4" s="1" t="str">
+        <v/>
+      </c>
+      <c r="N4" s="2">
         <v>43679</v>
       </c>
-      <c r="O2" s="1" t="str">
+      <c r="O4" s="1" t="str">
         <v>Resecció Menor (&lt;3 segm)</v>
       </c>
-      <c r="P2" s="1" t="str">
+      <c r="P4" s="1" t="str">
         <v>bisegm 2/3 i 4 RL r0 una d'elles</v>
       </c>
-      <c r="Q2" s="1" t="str">
+      <c r="Q4" s="1" t="str">
         <v>Oberta</v>
       </c>
-      <c r="R2" s="1" t="str">
-        <v>No</v>
-      </c>
-      <c r="S2" s="1" t="str">
-        <v>No</v>
-      </c>
-      <c r="T2" s="1" t="str">
+      <c r="R4" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="S4" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="T4" s="1" t="str">
         <v>Impressió R1</v>
       </c>
-      <c r="U2" s="1" t="str">
-        <v>Si</v>
-      </c>
-      <c r="V2" s="1" t="str">
-        <v>No</v>
-      </c>
-      <c r="W2" s="1" t="str">
-        <v>No</v>
-      </c>
-      <c r="X2" s="1" t="str">
-        <v>No</v>
-      </c>
-      <c r="Y2" s="1" t="str">
-        <v/>
-      </c>
-      <c r="Z2" s="1" t="str">
-        <v/>
-      </c>
-      <c r="AA2" s="1" t="str">
-        <v/>
-      </c>
-      <c r="AB2" s="1" t="str">
-        <v/>
-      </c>
-      <c r="AC2" s="1">
+      <c r="U4" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="V4" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="W4" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="X4" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Y4" s="1" t="str">
+        <v/>
+      </c>
+      <c r="Z4" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AA4" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AB4" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AC4" s="1">
         <v>7</v>
       </c>
-      <c r="AD2" s="1">
+      <c r="AD4" s="1">
         <v>2.8</v>
       </c>
-      <c r="AE2" s="1">
+      <c r="AE4" s="1">
         <v>0</v>
       </c>
-      <c r="AF2" s="1" t="str">
-        <v>Si</v>
-      </c>
-      <c r="AG2" s="1" t="str">
+      <c r="AF4" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AG4" s="1" t="str">
         <v>aquamantis</v>
       </c>
-      <c r="AH2" s="2">
+      <c r="AH4" s="2">
         <v>44525</v>
       </c>
-      <c r="AI2" s="1" t="str">
-        <v>No</v>
-      </c>
-      <c r="AJ2" s="1" t="str">
-        <v/>
-      </c>
-      <c r="AK2" s="1" t="str">
+      <c r="AI4" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AJ4" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AK4" s="1" t="str">
         <v>Viu</v>
       </c>
-      <c r="AL2" s="1" t="str">
-        <v/>
-      </c>
-      <c r="AM2" s="1" t="str">
-        <v/>
-      </c>
-      <c r="AN2" s="1" t="str">
-        <v/>
-      </c>
-      <c r="AO2" s="1" t="str">
-        <v/>
-      </c>
-      <c r="AP2" s="1" t="str">
-        <v/>
-      </c>
-      <c r="AQ2" s="1" t="str">
-        <v/>
-      </c>
-      <c r="AR2" s="1" t="str">
-        <v/>
-      </c>
-      <c r="AS2" s="1" t="str">
-        <v/>
-      </c>
-      <c r="AT2" s="1" t="str">
-        <v>Si</v>
-      </c>
-      <c r="AU2" s="1" t="str">
-        <v>Si</v>
-      </c>
-      <c r="AV2" s="1" t="str">
-        <v>Si</v>
-      </c>
-      <c r="AW2" s="2">
-        <v>44600.41150771991</v>
-      </c>
-      <c r="AX2" s="1" t="str">
+      <c r="AL4" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AM4" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AN4" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AO4" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AP4" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AQ4" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AR4" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AS4" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AT4" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AU4" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AV4" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AW4" s="2">
+        <v>44601.37257071759</v>
+      </c>
+      <c r="AX4" s="1" t="str">
         <v>Falta alguna variable, revisar</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="1" t="str">
+    <row r="5">
+      <c r="A5" s="1" t="str">
+        <v>Resecció/ns limitada/es</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1669</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1529</v>
+      </c>
+      <c r="D5" s="1" t="str">
+        <v>Salvador</v>
+      </c>
+      <c r="E5" s="1" t="str">
+        <v>Monte</v>
+      </c>
+      <c r="F5" s="1" t="str">
+        <v>Peiro</v>
+      </c>
+      <c r="G5" s="1">
+        <v>13005406</v>
+      </c>
+      <c r="H5" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="I5" s="1" t="str">
+        <v>Home</v>
+      </c>
+      <c r="J5" s="1" t="str">
+        <v>60</v>
+      </c>
+      <c r="K5" s="1" t="str">
+        <v/>
+      </c>
+      <c r="L5" s="2">
+        <v>43525</v>
+      </c>
+      <c r="M5" s="1" t="str">
+        <v/>
+      </c>
+      <c r="N5" s="2">
+        <v>43679</v>
+      </c>
+      <c r="O5" s="1" t="str">
+        <v>Resecció Menor (&lt;3 segm)</v>
+      </c>
+      <c r="P5" s="1" t="str">
+        <v>bisegm 2/3 i 4 RL r0 una d'elles</v>
+      </c>
+      <c r="Q5" s="1" t="str">
+        <v>Oberta</v>
+      </c>
+      <c r="R5" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="S5" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="T5" s="1" t="str">
+        <v>Impressió R1</v>
+      </c>
+      <c r="U5" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="V5" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="W5" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="X5" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Y5" s="1" t="str">
+        <v/>
+      </c>
+      <c r="Z5" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AA5" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AB5" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AC5" s="1">
+        <v>7</v>
+      </c>
+      <c r="AD5" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="AE5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF5" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AG5" s="1" t="str">
+        <v>aquamantis</v>
+      </c>
+      <c r="AH5" s="2">
+        <v>44525</v>
+      </c>
+      <c r="AI5" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AJ5" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AK5" s="1" t="str">
+        <v>Viu</v>
+      </c>
+      <c r="AL5" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AM5" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AN5" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AO5" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AP5" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AQ5" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AR5" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AS5" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AT5" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AU5" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AV5" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AW5" s="2">
+        <v>44601.37490358797</v>
+      </c>
+      <c r="AX5" s="1" t="str">
+        <v>Falta alguna variable, revisar</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="str">
         <v>Hepatectomia dreta</v>
       </c>
-      <c r="B3" s="1">
-        <v>1695</v>
-      </c>
-      <c r="D3" s="1" t="str">
-        <v>Jordi</v>
-      </c>
-      <c r="E3" s="1" t="str">
-        <v>Morillas2</v>
-      </c>
-      <c r="F3" s="1" t="str">
-        <v>Esteban2</v>
-      </c>
-      <c r="G3" s="1">
-        <v>13296015</v>
-      </c>
-      <c r="H3" s="1" t="str">
-        <v>No</v>
-      </c>
-      <c r="I3" s="1" t="str">
-        <v/>
-      </c>
-      <c r="J3" s="1" t="str">
-        <v/>
-      </c>
-      <c r="K3" s="1" t="str">
-        <v>79</v>
-      </c>
-      <c r="L3" s="2">
-        <v>43446</v>
-      </c>
-      <c r="M3" s="1" t="str">
-        <v>No</v>
-      </c>
-      <c r="N3" s="2">
-        <v>43858</v>
-      </c>
-      <c r="O3" s="1" t="str">
+      <c r="B6" s="1">
+        <v>1668</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1528</v>
+      </c>
+      <c r="D6" s="1" t="str">
+        <v>Juan P</v>
+      </c>
+      <c r="E6" s="1" t="str">
+        <v>Montes</v>
+      </c>
+      <c r="F6" s="1" t="str">
+        <v>Alcañiz</v>
+      </c>
+      <c r="G6" s="1">
+        <v>18493694</v>
+      </c>
+      <c r="H6" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="I6" s="1" t="str">
+        <v>Home</v>
+      </c>
+      <c r="J6" s="1" t="str">
+        <v>53</v>
+      </c>
+      <c r="K6" s="1" t="str">
+        <v>80</v>
+      </c>
+      <c r="L6" s="2">
+        <v>43416</v>
+      </c>
+      <c r="M6" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="N6" s="2">
+        <v>43677</v>
+      </c>
+      <c r="O6" s="1" t="str">
         <v>Resecció Major (&gt;= 3 segm)</v>
       </c>
-      <c r="P3" s="1" t="str">
-        <v>hepatectomia dreta</v>
-      </c>
-      <c r="Q3" s="1" t="str">
+      <c r="P6" s="1" t="str">
+        <v>Hepatectomia dreta</v>
+      </c>
+      <c r="Q6" s="1" t="str">
         <v>Oberta</v>
       </c>
-      <c r="R3" s="1" t="str">
-        <v>Si, com a primer temps quirúrgic</v>
-      </c>
-      <c r="S3" s="1" t="str">
-        <v>No</v>
-      </c>
-      <c r="T3" s="1" t="str">
+      <c r="R6" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="S6" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="T6" s="1" t="str">
+        <v>Impressió R0</v>
+      </c>
+      <c r="U6" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="V6" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="W6" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="X6" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Y6" s="1" t="str">
+        <v/>
+      </c>
+      <c r="Z6" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AA6" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AB6" s="1" t="str">
+        <v>II</v>
+      </c>
+      <c r="AC6" s="1">
+        <v>2</v>
+      </c>
+      <c r="AD6" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="AE6" s="1">
+        <v>1</v>
+      </c>
+      <c r="AF6" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AG6" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AH6" s="2">
+        <v>44462</v>
+      </c>
+      <c r="AI6" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AJ6" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AK6" s="1" t="str">
+        <v>Viu</v>
+      </c>
+      <c r="AL6" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AM6" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AN6" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AO6" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AP6" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AQ6" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AR6" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AS6" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AT6" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AU6" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AV6" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AW6" s="2">
+        <v>44601.37493761574</v>
+      </c>
+      <c r="AX6" s="1" t="str">
+        <v xml:space="preserve">unable to complete promise all for CMD data after condition CMD = true, error message: </v>
+      </c>
+      <c r="AY6" s="1">
+        <v>172</v>
+      </c>
+      <c r="AZ6" s="1">
+        <v>27</v>
+      </c>
+      <c r="BA6" s="1">
+        <v>3</v>
+      </c>
+      <c r="BB6" s="1">
+        <v>6</v>
+      </c>
+      <c r="BC6" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="BD6" s="1">
+        <v>21</v>
+      </c>
+      <c r="BE6" s="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="str">
+        <v>Hepatectomia major + resecció contralateral</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1639</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1502</v>
+      </c>
+      <c r="D7" s="1" t="str">
+        <v>JOSE</v>
+      </c>
+      <c r="E7" s="1" t="str">
+        <v>MORALES</v>
+      </c>
+      <c r="F7" s="1" t="str">
+        <v>PEREZ</v>
+      </c>
+      <c r="G7" s="1">
+        <v>13804187</v>
+      </c>
+      <c r="H7" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="I7" s="1" t="str">
+        <v>Home</v>
+      </c>
+      <c r="J7" s="1" t="str">
+        <v>58</v>
+      </c>
+      <c r="K7" s="1" t="str">
+        <v>77</v>
+      </c>
+      <c r="L7" s="2">
+        <v>42827</v>
+      </c>
+      <c r="M7" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="N7" s="2">
+        <v>43539</v>
+      </c>
+      <c r="O7" s="1" t="str">
+        <v>Resecció Major (&gt;= 3 segm)</v>
+      </c>
+      <c r="P7" s="1" t="str">
+        <v>hepat esquerra i rl 7</v>
+      </c>
+      <c r="Q7" s="1" t="str">
+        <v>1er temps (mobilització)</v>
+      </c>
+      <c r="R7" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="S7" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="T7" s="1" t="str">
+        <v>Impressió R0</v>
+      </c>
+      <c r="U7" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="V7" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="W7" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="X7" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Y7" s="1" t="str">
+        <v/>
+      </c>
+      <c r="Z7" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AA7" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AB7" s="1" t="str">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="1">
+        <v>3</v>
+      </c>
+      <c r="AD7" s="1">
+        <v>4</v>
+      </c>
+      <c r="AE7" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="AF7" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AG7" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AH7" s="2">
+        <v>44301</v>
+      </c>
+      <c r="AI7" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AJ7" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AK7" s="1" t="str">
+        <v>Viu</v>
+      </c>
+      <c r="AL7" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AM7" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AN7" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AO7" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AP7" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AQ7" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AR7" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AS7" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AT7" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AU7" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AV7" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AW7" s="2">
+        <v>44601.37493773148</v>
+      </c>
+      <c r="AX7" s="1" t="str">
+        <v xml:space="preserve">unable to complete promise all for CMD data after condition CMD = true, error message: </v>
+      </c>
+      <c r="AY7" s="1">
+        <v>166</v>
+      </c>
+      <c r="AZ7" s="1">
+        <v>28</v>
+      </c>
+      <c r="BA7" s="1">
+        <v>2</v>
+      </c>
+      <c r="BB7" s="1">
+        <v>2</v>
+      </c>
+      <c r="BC7" s="1">
+        <v>4</v>
+      </c>
+      <c r="BD7" s="1">
+        <v>0</v>
+      </c>
+      <c r="BE7" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="str">
+        <v>Resecció/ns limitada/es</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1669</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1529</v>
+      </c>
+      <c r="D8" s="1" t="str">
+        <v>Salvador</v>
+      </c>
+      <c r="E8" s="1" t="str">
+        <v>Monte</v>
+      </c>
+      <c r="F8" s="1" t="str">
+        <v>Peiro</v>
+      </c>
+      <c r="G8" s="1">
+        <v>13005406</v>
+      </c>
+      <c r="H8" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="I8" s="1" t="str">
+        <v>Home</v>
+      </c>
+      <c r="J8" s="1" t="str">
+        <v>60</v>
+      </c>
+      <c r="K8" s="1" t="str">
+        <v/>
+      </c>
+      <c r="L8" s="2">
+        <v>43525</v>
+      </c>
+      <c r="M8" s="1" t="str">
+        <v/>
+      </c>
+      <c r="N8" s="2">
+        <v>43679</v>
+      </c>
+      <c r="O8" s="1" t="str">
+        <v>Resecció Menor (&lt;3 segm)</v>
+      </c>
+      <c r="P8" s="1" t="str">
+        <v>bisegm 2/3 i 4 RL r0 una d'elles</v>
+      </c>
+      <c r="Q8" s="1" t="str">
+        <v>Oberta</v>
+      </c>
+      <c r="R8" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="S8" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="T8" s="1" t="str">
         <v>Impressió R1</v>
       </c>
-      <c r="U3" s="1" t="str">
-        <v>No</v>
-      </c>
-      <c r="V3" s="1" t="str">
-        <v>Si</v>
-      </c>
-      <c r="W3" s="1" t="str">
-        <v>No</v>
-      </c>
-      <c r="X3" s="1" t="str">
-        <v>No</v>
-      </c>
-      <c r="Y3" s="1" t="str">
-        <v/>
-      </c>
-      <c r="Z3" s="1" t="str">
-        <v/>
-      </c>
-      <c r="AA3" s="1" t="str">
-        <v>Si</v>
-      </c>
-      <c r="AB3" s="1" t="str">
-        <v>IIIb</v>
-      </c>
-      <c r="AC3" s="1">
-        <v>1</v>
-      </c>
-      <c r="AD3" s="1">
-        <v>3</v>
-      </c>
-      <c r="AE3" s="1">
+      <c r="U8" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="V8" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="W8" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="X8" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Y8" s="1" t="str">
+        <v/>
+      </c>
+      <c r="Z8" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AA8" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AB8" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AC8" s="1">
+        <v>7</v>
+      </c>
+      <c r="AD8" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="AE8" s="1">
         <v>0</v>
       </c>
-      <c r="AF3" s="1" t="str">
-        <v>Si</v>
-      </c>
-      <c r="AG3" s="1" t="str">
-        <v>ampliacio quirurgica</v>
-      </c>
-      <c r="AH3" s="2">
-        <v>43983</v>
-      </c>
-      <c r="AI3" s="1" t="str">
-        <v>No</v>
-      </c>
-      <c r="AJ3" s="1" t="str">
-        <v>No</v>
-      </c>
-      <c r="AK3" s="1" t="str">
+      <c r="AF8" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AG8" s="1" t="str">
+        <v>aquamantis</v>
+      </c>
+      <c r="AH8" s="2">
+        <v>44525</v>
+      </c>
+      <c r="AI8" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AJ8" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AK8" s="1" t="str">
         <v>Viu</v>
       </c>
-      <c r="AL3" s="1" t="str">
-        <v>Si</v>
-      </c>
-      <c r="AM3" s="1" t="str">
-        <v/>
-      </c>
-      <c r="AN3" s="1" t="str">
-        <v>Si</v>
-      </c>
-      <c r="AO3" s="1" t="str">
-        <v>No</v>
-      </c>
-      <c r="AP3" s="1" t="str">
-        <v>No</v>
-      </c>
-      <c r="AQ3" s="1" t="str">
-        <v>Si</v>
-      </c>
-      <c r="AR3" s="1" t="str">
-        <v>No</v>
-      </c>
-      <c r="AS3" s="1" t="str">
-        <v>oclusió, peritonitis fecaoidea</v>
-      </c>
-      <c r="AT3" s="1" t="str">
-        <v>No</v>
-      </c>
-      <c r="AU3" s="1" t="str">
-        <v>No</v>
-      </c>
-      <c r="AV3" s="1" t="str">
-        <v>No</v>
-      </c>
-      <c r="AW3" s="2">
-        <v>44600.4125950463</v>
-      </c>
-      <c r="AX3" s="1" t="str">
+      <c r="AL8" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AM8" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AN8" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AO8" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AP8" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AQ8" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AR8" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AS8" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AT8" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AU8" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AV8" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AW8" s="2">
+        <v>44601.375009525465</v>
+      </c>
+      <c r="AX8" s="1" t="str">
         <v>Falta alguna variable, revisar</v>
       </c>
-      <c r="AY3" s="1">
-        <v>178</v>
-      </c>
-      <c r="AZ3" s="1">
-        <v>25</v>
-      </c>
-      <c r="BA3" s="1">
-        <v>3</v>
-      </c>
-      <c r="BB3" s="1">
-        <v>1</v>
-      </c>
-      <c r="BC3" s="1">
-        <v>3</v>
-      </c>
-      <c r="BD3" s="1">
-        <v>61</v>
-      </c>
-      <c r="BE3" s="1">
-        <v>55</v>
-      </c>
-      <c r="BF3" s="1">
-        <v>2</v>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="str">
+        <v>Resecció/ns limitada/es</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1669</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1529</v>
+      </c>
+      <c r="D9" s="1" t="str">
+        <v>Salvador</v>
+      </c>
+      <c r="E9" s="1" t="str">
+        <v>Monte</v>
+      </c>
+      <c r="F9" s="1" t="str">
+        <v>Peiro</v>
+      </c>
+      <c r="G9" s="1">
+        <v>13005406</v>
+      </c>
+      <c r="H9" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="I9" s="1" t="str">
+        <v>Home</v>
+      </c>
+      <c r="J9" s="1" t="str">
+        <v>60</v>
+      </c>
+      <c r="K9" s="1" t="str">
+        <v/>
+      </c>
+      <c r="L9" s="2">
+        <v>43525</v>
+      </c>
+      <c r="M9" s="1" t="str">
+        <v/>
+      </c>
+      <c r="N9" s="2">
+        <v>43679</v>
+      </c>
+      <c r="O9" s="1" t="str">
+        <v>Resecció Menor (&lt;3 segm)</v>
+      </c>
+      <c r="P9" s="1" t="str">
+        <v>bisegm 2/3 i 4 RL r0 una d'elles</v>
+      </c>
+      <c r="Q9" s="1" t="str">
+        <v>Oberta</v>
+      </c>
+      <c r="R9" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="S9" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="T9" s="1" t="str">
+        <v>Impressió R1</v>
+      </c>
+      <c r="U9" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="V9" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="W9" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="X9" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Y9" s="1" t="str">
+        <v/>
+      </c>
+      <c r="Z9" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AA9" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AB9" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AC9" s="1">
+        <v>7</v>
+      </c>
+      <c r="AD9" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="AE9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF9" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AG9" s="1" t="str">
+        <v>aquamantis</v>
+      </c>
+      <c r="AH9" s="2">
+        <v>44525</v>
+      </c>
+      <c r="AI9" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AJ9" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AK9" s="1" t="str">
+        <v>Viu</v>
+      </c>
+      <c r="AL9" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AM9" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AN9" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AO9" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AP9" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AQ9" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AR9" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AS9" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AT9" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AU9" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AV9" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AW9" s="2">
+        <v>44601.37611287037</v>
+      </c>
+      <c r="AX9" s="1" t="str">
+        <v>Falta alguna variable, revisar</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:BF3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:BE9"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>